<commit_message>
Update data source for "2022-CUMCM-Problem-C"
</commit_message>
<xml_diff>
--- a/2022-CUMCM/Problem C/attachment/附件.xlsx
+++ b/2022-CUMCM/Problem C/attachment/附件.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Python Project\mathworks\2022数模国赛\C题\附件\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Python Project\mathworks\2022-CUMCM\Problem C\attachment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{726211EA-F98A-44D9-9478-BFBFEEE6128C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09A324C3-698C-49E6-8F38-867BB726FC51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>